<commit_message>
Updated pick and place file
</commit_message>
<xml_diff>
--- a/fab/BOM_JLCSMT.xlsx
+++ b/fab/BOM_JLCSMT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rduarte\Dropbox\data\diptrace\My Projects\Zest attiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF8D795-0741-4E81-9C34-636F7E4598EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4FA958-D7AD-499F-9569-856476B9B3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-84" yWindow="0" windowWidth="11688" windowHeight="13044" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -194,10 +194,10 @@
     <t>C71136</t>
   </si>
   <si>
-    <t>SOT-89-3</t>
-  </si>
-  <si>
-    <t>78L05G-AB3-R</t>
+    <t>78L05G</t>
+  </si>
+  <si>
+    <t>UC_SOT89</t>
   </si>
 </sst>
 </file>
@@ -661,7 +661,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -728,13 +728,13 @@
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>42</v>

</xml_diff>